<commit_message>
Actualizando archivos bicicletas, subte y vehiculos
</commit_message>
<xml_diff>
--- a/bicicletas.xlsx
+++ b/bicicletas.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>AÑO_MES</t>
   </si>
   <si>
-    <t>TIPO</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
+    <t>BICICLETAS</t>
   </si>
   <si>
     <t>202001</t>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t>202106</t>
-  </si>
-  <si>
-    <t>BICICLETAS</t>
   </si>
 </sst>
 </file>
@@ -437,210 +431,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>159233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1">
-        <v>159233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>116965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1">
-        <v>116965</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>52951</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1">
-        <v>52951</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>20235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1">
-        <v>20235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>69707</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1">
-        <v>69707</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>98328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1">
-        <v>98328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1">
+        <v>248180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <v>248180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1">
+        <v>273719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1">
-        <v>273719</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1">
+        <v>323130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1">
-        <v>323130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>332410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1">
-        <v>332410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>308087</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1">
-        <v>308087</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1">
+        <v>277277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1">
-        <v>277277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1">
+        <v>312790</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1">
-        <v>312790</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1">
+        <v>300889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1">
-        <v>300889</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>235238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1">
-        <v>235238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1">
+        <v>193235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1">
-        <v>193235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="1">
         <v>9297</v>
       </c>
     </row>

</xml_diff>